<commit_message>
updated readme files and renamed a few files for consistency
</commit_message>
<xml_diff>
--- a/Growth_trait_analyses/Allometric_Relationships_Basic_20200712_ErindaleParkMilkweed.xlsx
+++ b/Growth_trait_analyses/Allometric_Relationships_Basic_20200712_ErindaleParkMilkweed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\Growth_trait_analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17E1B1CF-54E2-4D7F-895A-7AC0E28D8DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530D76F-684C-443C-B88B-EB8A84580A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84EAA4FE-CCB3-49DA-8517-BCBEB9C0DD90}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Plant</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>f = flowering</t>
+  </si>
+  <si>
+    <t>Height, stem width, weight, and flowering status were observed for 31 milkweed ramets, selected &gt;3 meters apart, at Erindale Park in Mississauga, Ontario, Canada, on 7/12/2020.</t>
   </si>
 </sst>
 </file>
@@ -3033,10 +3036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73281FAC-674B-4093-BC6B-CC4D503FC28B}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3296,7 +3299,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>19</v>
       </c>
@@ -3311,7 +3314,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>23</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>24</v>
       </c>
@@ -3345,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>15</v>
       </c>
@@ -3378,8 +3381,11 @@
       <c r="E21" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>1</v>
       </c>
@@ -3394,7 +3400,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>5</v>
       </c>
@@ -3409,7 +3415,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>26</v>
       </c>
@@ -3426,7 +3432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>14</v>
       </c>
@@ -3443,7 +3449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>13</v>
       </c>
@@ -3460,7 +3466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>3</v>
       </c>
@@ -3475,7 +3481,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>10</v>
       </c>
@@ -3492,7 +3498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>12</v>
       </c>
@@ -3509,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>17</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>11</v>
       </c>
@@ -3543,7 +3549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>16</v>
       </c>

</xml_diff>